<commit_message>
Cambio en la gramatica para permitir el uso de IDs para las expresiones de lista
</commit_message>
<xml_diff>
--- a/TAS.xlsx
+++ b/TAS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="10515" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="archivoTas" localSheetId="0">Hoja1!$A$1:$AA$21</definedName>
+    <definedName name="TAS" localSheetId="0">Hoja1!$A$1:$AA$22</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -20,8 +20,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="archivoTas" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr sourceFile="C:\Users\Rodrigo Romero\Desktop\Compu vieja\Facultad\Sintaxis y Semantica de los lenguajes\SyS\archivoTas.csv" decimal="," thousands=".">
+  <connection id="1" name="TAS" type="6" refreshedVersion="4" background="1" saveData="1">
+    <textPr sourceFile="C:\Users\Rodrigo Romero\Desktop\Compu vieja\Facultad\Sintaxis y Semantica de los lenguajes\SyS\TAS.txt" decimal="," thousands=".">
       <textFields count="27">
         <textField/>
         <textField/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="86">
   <si>
     <t>$</t>
   </si>
@@ -161,6 +161,9 @@
     <t>Oplista</t>
   </si>
   <si>
+    <t>Explistaoid</t>
+  </si>
+  <si>
     <t>Lista</t>
   </si>
   <si>
@@ -239,10 +242,16 @@
     <t>Explista --&gt; Oplista</t>
   </si>
   <si>
-    <t>Oplista --&gt; cons parentesis1 Exparit coma Explista parentesis2</t>
-  </si>
-  <si>
-    <t>Oplista --&gt; rest parentesis1 Explista parentesis2</t>
+    <t>Oplista --&gt; cons parentesis1 Exparit coma Explistaoid parentesis2</t>
+  </si>
+  <si>
+    <t>Oplista --&gt; rest parentesis1 Explistaoid parentesis2</t>
+  </si>
+  <si>
+    <t>Explistaoid --&gt; id</t>
+  </si>
+  <si>
+    <t>Explistaoid --&gt; Explista</t>
   </si>
   <si>
     <t>Lista --&gt; corchete1 Listanum corchete2</t>
@@ -266,7 +275,7 @@
     <t>Exparit --&gt; consent Exparit2</t>
   </si>
   <si>
-    <t>Exparit --&gt; first parentesis1 Explista parentesis2 Exparit2</t>
+    <t>Exparit --&gt; first parentesis1 Explistaoid parentesis2 Exparit2</t>
   </si>
   <si>
     <t>Exparit2 --&gt; &amp;epsilon</t>
@@ -302,7 +311,7 @@
     <t>Condicion --&gt; Exparit oprel Exparit</t>
   </si>
   <si>
-    <t>Condicion --&gt; null parentesis1 Explista parentesis2</t>
+    <t>Condicion --&gt; null parentesis1 Explistaoid parentesis2</t>
   </si>
   <si>
     <t>Ciclo --&gt; mientras Condicion hacer Programa fin</t>
@@ -358,7 +367,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="archivoTas" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="TAS" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -648,9 +657,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA21"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -660,7 +671,7 @@
     <col min="5" max="5" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
@@ -673,11 +684,11 @@
     <col min="18" max="18" width="55.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="46.5703125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -776,7 +787,7 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
         <v>27</v>
@@ -797,7 +808,7 @@
         <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M2" t="s">
         <v>27</v>
@@ -806,16 +817,16 @@
         <v>27</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="Q2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="R2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S2" t="s">
         <v>27</v>
@@ -850,37 +861,37 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
       </c>
       <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
         <v>49</v>
       </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>48</v>
-      </c>
       <c r="K3" t="s">
         <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M3" t="s">
         <v>27</v>
@@ -889,16 +900,16 @@
         <v>27</v>
       </c>
       <c r="O3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Q3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="R3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S3" t="s">
         <v>27</v>
@@ -942,7 +953,7 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
@@ -963,7 +974,7 @@
         <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M4" t="s">
         <v>27</v>
@@ -972,16 +983,16 @@
         <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S4" t="s">
         <v>27</v>
@@ -1058,7 +1069,7 @@
         <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q5" t="s">
         <v>27</v>
@@ -1114,7 +1125,7 @@
         <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H6" t="s">
         <v>27</v>
@@ -1141,7 +1152,7 @@
         <v>27</v>
       </c>
       <c r="P6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q6" t="s">
         <v>27</v>
@@ -1153,22 +1164,22 @@
         <v>27</v>
       </c>
       <c r="T6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="U6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V6" t="s">
         <v>27</v>
       </c>
       <c r="W6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="X6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Y6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Z6" t="s">
         <v>27</v>
@@ -1245,13 +1256,13 @@
         <v>27</v>
       </c>
       <c r="W7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="X7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Y7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Z7" t="s">
         <v>27</v>
@@ -1331,10 +1342,10 @@
         <v>27</v>
       </c>
       <c r="X8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Y8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Z8" t="s">
         <v>27</v>
@@ -1390,7 +1401,7 @@
         <v>27</v>
       </c>
       <c r="P9" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="Q9" t="s">
         <v>27</v>
@@ -1411,13 +1422,13 @@
         <v>27</v>
       </c>
       <c r="W9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="X9" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Y9" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="Z9" t="s">
         <v>27</v>
@@ -1485,7 +1496,7 @@
         <v>27</v>
       </c>
       <c r="T10" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="U10" t="s">
         <v>27</v>
@@ -1494,7 +1505,7 @@
         <v>27</v>
       </c>
       <c r="W10" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="X10" t="s">
         <v>27</v>
@@ -1547,7 +1558,7 @@
         <v>27</v>
       </c>
       <c r="M11" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="N11" t="s">
         <v>27</v>
@@ -1568,13 +1579,13 @@
         <v>27</v>
       </c>
       <c r="T11" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="U11" t="s">
         <v>27</v>
       </c>
       <c r="V11" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="W11" t="s">
         <v>27</v>
@@ -1612,7 +1623,7 @@
         <v>27</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="H12" t="s">
         <v>27</v>
@@ -1630,7 +1641,7 @@
         <v>27</v>
       </c>
       <c r="M12" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="N12" t="s">
         <v>27</v>
@@ -1639,7 +1650,7 @@
         <v>27</v>
       </c>
       <c r="P12" t="s">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="Q12" t="s">
         <v>27</v>
@@ -1651,13 +1662,13 @@
         <v>27</v>
       </c>
       <c r="T12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V12" t="s">
         <v>68</v>
-      </c>
-      <c r="U12" t="s">
-        <v>69</v>
-      </c>
-      <c r="V12" t="s">
-        <v>27</v>
       </c>
       <c r="W12" t="s">
         <v>27</v>
@@ -1686,44 +1697,44 @@
         <v>27</v>
       </c>
       <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" t="s">
+        <v>27</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" t="s">
+        <v>27</v>
+      </c>
+      <c r="O13" t="s">
+        <v>27</v>
+      </c>
+      <c r="P13" t="s">
         <v>70</v>
       </c>
-      <c r="E13" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" t="s">
-        <v>27</v>
-      </c>
-      <c r="K13" t="s">
-        <v>70</v>
-      </c>
-      <c r="L13" t="s">
-        <v>27</v>
-      </c>
-      <c r="M13" t="s">
-        <v>70</v>
-      </c>
-      <c r="N13" t="s">
-        <v>27</v>
-      </c>
-      <c r="O13" t="s">
-        <v>27</v>
-      </c>
-      <c r="P13" t="s">
-        <v>27</v>
-      </c>
       <c r="Q13" t="s">
         <v>27</v>
       </c>
@@ -1731,13 +1742,13 @@
         <v>27</v>
       </c>
       <c r="S13" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" t="s">
         <v>71</v>
       </c>
-      <c r="T13" t="s">
-        <v>27</v>
-      </c>
       <c r="U13" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="V13" t="s">
         <v>27</v>
@@ -1755,7 +1766,7 @@
         <v>27</v>
       </c>
       <c r="AA13" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
@@ -1769,13 +1780,13 @@
         <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
         <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="G14" t="s">
         <v>27</v>
@@ -1784,19 +1795,19 @@
         <v>27</v>
       </c>
       <c r="I14" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="J14" t="s">
         <v>27</v>
       </c>
       <c r="K14" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="L14" t="s">
         <v>27</v>
       </c>
       <c r="M14" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="N14" t="s">
         <v>27</v>
@@ -1808,37 +1819,37 @@
         <v>27</v>
       </c>
       <c r="Q14" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="R14" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" t="s">
+        <v>74</v>
+      </c>
+      <c r="T14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" t="s">
+        <v>27</v>
+      </c>
+      <c r="V14" t="s">
+        <v>27</v>
+      </c>
+      <c r="W14" t="s">
+        <v>27</v>
+      </c>
+      <c r="X14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA14" t="s">
         <v>73</v>
-      </c>
-      <c r="S14" t="s">
-        <v>27</v>
-      </c>
-      <c r="T14" t="s">
-        <v>27</v>
-      </c>
-      <c r="U14" t="s">
-        <v>27</v>
-      </c>
-      <c r="V14" t="s">
-        <v>27</v>
-      </c>
-      <c r="W14" t="s">
-        <v>27</v>
-      </c>
-      <c r="X14" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
@@ -1891,10 +1902,10 @@
         <v>27</v>
       </c>
       <c r="Q15" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="R15" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S15" t="s">
         <v>27</v>
@@ -1974,10 +1985,10 @@
         <v>27</v>
       </c>
       <c r="Q16" t="s">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="R16" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="S16" t="s">
         <v>27</v>
@@ -2051,13 +2062,13 @@
         <v>27</v>
       </c>
       <c r="O17" t="s">
-        <v>76</v>
+        <v>27</v>
       </c>
       <c r="P17" t="s">
         <v>27</v>
       </c>
       <c r="Q17" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="R17" t="s">
         <v>27</v>
@@ -2125,7 +2136,7 @@
         <v>27</v>
       </c>
       <c r="L18" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="M18" t="s">
         <v>27</v>
@@ -2134,7 +2145,7 @@
         <v>27</v>
       </c>
       <c r="O18" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="P18" t="s">
         <v>27</v>
@@ -2181,7 +2192,7 @@
         <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
         <v>27</v>
@@ -2202,13 +2213,13 @@
         <v>27</v>
       </c>
       <c r="J19" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="K19" t="s">
         <v>27</v>
       </c>
       <c r="L19" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="M19" t="s">
         <v>27</v>
@@ -2264,7 +2275,7 @@
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>81</v>
       </c>
       <c r="D20" t="s">
         <v>27</v>
@@ -2276,16 +2287,16 @@
         <v>27</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="H20" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="I20" t="s">
         <v>27</v>
       </c>
       <c r="J20" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="K20" t="s">
         <v>27</v>
@@ -2303,7 +2314,7 @@
         <v>27</v>
       </c>
       <c r="P20" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="Q20" t="s">
         <v>27</v>
@@ -2315,10 +2326,10 @@
         <v>27</v>
       </c>
       <c r="T20" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="U20" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="V20" t="s">
         <v>27</v>
@@ -2353,16 +2364,16 @@
         <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
         <v>27</v>
       </c>
       <c r="G21" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="I21" t="s">
         <v>27</v>
@@ -2386,7 +2397,7 @@
         <v>27</v>
       </c>
       <c r="P21" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="Q21" t="s">
         <v>27</v>
@@ -2398,10 +2409,10 @@
         <v>27</v>
       </c>
       <c r="T21" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="U21" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="V21" t="s">
         <v>27</v>
@@ -2419,6 +2430,89 @@
         <v>27</v>
       </c>
       <c r="AA21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" t="s">
+        <v>27</v>
+      </c>
+      <c r="N22" t="s">
+        <v>27</v>
+      </c>
+      <c r="O22" t="s">
+        <v>27</v>
+      </c>
+      <c r="P22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>27</v>
+      </c>
+      <c r="R22" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" t="s">
+        <v>27</v>
+      </c>
+      <c r="T22" t="s">
+        <v>27</v>
+      </c>
+      <c r="U22" t="s">
+        <v>27</v>
+      </c>
+      <c r="V22" t="s">
+        <v>27</v>
+      </c>
+      <c r="W22" t="s">
+        <v>27</v>
+      </c>
+      <c r="X22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA22" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>